<commit_message>
Updated PropertyCards to use a superclass-subclass structure.
New classes are BoardPiece, ColouredProperty, FreeParkingPiece, GoPiece, GoToJailPiece, JailPiece,OpportunityKnocksPiece, PotLuckPiece, Property, StationProperty, TaxPiece and UtilityProperty

Updated classes are GameLoop, PropertyTycoon, Bank and Player. (Fixes for updated arraylist from PropertyCards to the new structure.
</commit_message>
<xml_diff>
--- a/PropertyTycoon/src/main/java/resources/PropertyTycoonBoardData.xlsx
+++ b/PropertyTycoon/src/main/java/resources/PropertyTycoonBoardData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Desktop\SWE2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankee\Documents\UNIVERSITY\YEAR 2\SWE\PropertyTycoon\PropertyTycoon\src\main\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0837D3C-0F55-42D0-AA58-E50F46BFD7A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14580" windowHeight="8370" xr2:uid="{3AB37EF7-9957-4EAE-A376-EF9CBBC9245A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3AB37EF7-9957-4EAE-A376-EF9CBBC9245A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -680,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{194933F7-920A-45E1-89BC-1AB0AFB7405E}">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1840,7 +1841,7 @@
       <c r="B41" t="s">
         <v>28</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>20</v>
       </c>
       <c r="F41" t="s">

</xml_diff>